<commit_message>
clean up sample data
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Documents\Stuff\Logic\Coding Projects\lisser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CAF1946-B2BD-458F-903E-E81D6C721078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421770A4-8F15-4E33-AA27-E2E7E9FC6999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -178,9 +177,6 @@
   </si>
   <si>
     <t>_redacted_</t>
-  </si>
-  <si>
-    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -191,7 +187,7 @@
     <numFmt numFmtId="164" formatCode="m/d;@"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,12 +199,6 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -225,7 +215,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -251,17 +241,6 @@
         <color theme="1"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right/>
       <top style="thin">
         <color theme="1"/>
       </top>
@@ -275,23 +254,22 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="m/d;@"/>
       <fill>
@@ -315,100 +293,6 @@
         <horizontal/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -429,31 +313,15 @@
     <sortCondition ref="A1:A95"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Description"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Vendor"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Category"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Price" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Price" dataDxfId="0"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Is Food"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Controllable"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A911DC3C-FA4C-4527-9662-3E2BD75E264A}" name="Table3" displayName="Table3" ref="A1:B95" totalsRowShown="0" dataDxfId="2" tableBorderDxfId="4">
-  <autoFilter ref="A1:B95" xr:uid="{A911DC3C-FA4C-4527-9662-3E2BD75E264A}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B95">
-    <sortCondition ref="B1:B95"/>
-  </sortState>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{AC37F961-34F0-45E8-B984-00213DE133FC}" name="Date" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{6FCA42A8-F454-4965-8DB0-37B5B16651F9}" name="Column1" dataDxfId="1">
-      <calculatedColumnFormula>RAND()</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -776,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A95" sqref="A2:A95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -816,88 +684,88 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3">
-        <v>45392</v>
+        <v>45292</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E2" s="2">
-        <v>51.03421481904099</v>
+        <v>17.147002791824256</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="4">
-        <v>45389</v>
+      <c r="A3" s="3">
+        <v>45311</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>21.525176317465011</v>
+        <v>50.089501984960542</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="3">
-        <v>45595</v>
+      <c r="A4" s="4">
+        <v>45311</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
         <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2">
-        <v>6.8664125929764026</v>
+        <v>23.170220279194677</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="3">
-        <v>45394</v>
+      <c r="A5" s="4">
+        <v>45315</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
         <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2">
-        <v>52.128344351505071</v>
+        <v>18.209604367663978</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -907,11 +775,11 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="4">
-        <v>45474</v>
+      <c r="A6" s="3">
+        <v>45317</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
         <v>47</v>
@@ -920,7 +788,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="2">
-        <v>32.529640875787123</v>
+        <v>546.34269896948445</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -930,31 +798,31 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="3">
-        <v>45547</v>
+      <c r="A7" s="4">
+        <v>45321</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
         <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E7" s="2">
-        <v>19.033404509807344</v>
+        <v>66.682283323879389</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="4">
-        <v>45515</v>
+      <c r="A8" s="3">
+        <v>45322</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -966,7 +834,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>45.542571114625908</v>
+        <v>9.7536737962057725</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -976,100 +844,100 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="3">
-        <v>45395</v>
+      <c r="A9" s="4">
+        <v>45323</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
         <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2">
-        <v>18.449348228187279</v>
+        <v>23.859230634878017</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="3">
-        <v>45322</v>
+        <v>45332</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
         <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E10" s="2">
-        <v>9.7536737962057725</v>
+        <v>24.677305430093984</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4">
-        <v>45642</v>
+        <v>45336</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
         <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E11" s="2">
-        <v>35.881275421039959</v>
+        <v>4.1295821605673417</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="3">
-        <v>45478</v>
+        <v>45350</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
         <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E12" s="2">
-        <v>16.073972115983096</v>
+        <v>67.686150075286932</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="4">
-        <v>45395</v>
+        <v>45353</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
@@ -1081,7 +949,7 @@
         <v>8</v>
       </c>
       <c r="E13" s="2">
-        <v>50.319058517747656</v>
+        <v>8.4678212748500812</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -1091,184 +959,184 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="4">
-        <v>45632</v>
+      <c r="A14" s="3">
+        <v>45368</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E14" s="2">
-        <v>33.706145994917662</v>
+        <v>34.412227678898994</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="4">
-        <v>45552</v>
+        <v>45379</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
         <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E15" s="2">
-        <v>45.124918956005892</v>
+        <v>91.115032457869006</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="3">
-        <v>45447</v>
+        <v>45380</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
         <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E16" s="2">
-        <v>21.17005254480171</v>
+        <v>61.350532464411664</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="4">
-        <v>45462</v>
+        <v>45389</v>
       </c>
       <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="2">
+        <v>21.525176317465011</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="3">
+        <v>45392</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="2">
+        <v>51.03421481904099</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="4">
+        <v>45393</v>
+      </c>
+      <c r="B19" t="s">
         <v>27</v>
       </c>
-      <c r="C17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="2">
-        <v>6.1362243634941409</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="4">
-        <v>45457</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="2">
-        <v>9.0713740385982007</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="3">
-        <v>45543</v>
-      </c>
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
       <c r="E19" s="2">
-        <v>8.218023793872284</v>
+        <v>3.6981094178656995</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="3">
-        <v>45627</v>
+        <v>45394</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
         <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E20" s="2">
-        <v>55.806989867356052</v>
+        <v>52.128344351505071</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="3">
-        <v>45458</v>
+        <v>45395</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
         <v>47</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E21" s="2">
-        <v>4.4450988443080242</v>
+        <v>18.449348228187279</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1276,56 +1144,56 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="4">
-        <v>45540</v>
+        <v>45395</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="C22" t="s">
         <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E22" s="2">
-        <v>10.843589715267399</v>
+        <v>50.319058517747656</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="4">
-        <v>45653</v>
+        <v>45396</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C23" t="s">
         <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E23" s="2">
-        <v>4.5444022945078419</v>
+        <v>60.015682920995474</v>
       </c>
       <c r="F23">
         <v>1</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="3">
-        <v>45514</v>
+        <v>45402</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
         <v>47</v>
@@ -1334,7 +1202,7 @@
         <v>11</v>
       </c>
       <c r="E24" s="2">
-        <v>47.202743940079138</v>
+        <v>138.2147422166174</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1344,184 +1212,184 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="3">
-        <v>45572</v>
+      <c r="A25" s="4">
+        <v>45406</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
         <v>47</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E25" s="2">
-        <v>18.005409657329089</v>
+        <v>59.465543593581948</v>
       </c>
       <c r="F25">
         <v>1</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="3">
-        <v>45593</v>
+        <v>45412</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C26" t="s">
         <v>47</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E26" s="2">
-        <v>47.674742913663458</v>
+        <v>29.286465301629605</v>
       </c>
       <c r="F26">
         <v>0</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="3">
-        <v>45292</v>
+      <c r="A27" s="4">
+        <v>45419</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
         <v>47</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E27" s="2">
-        <v>17.147002791824256</v>
+        <v>25.568377219304327</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="3">
-        <v>45350</v>
+        <v>45423</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
         <v>47</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E28" s="2">
-        <v>67.686150075286932</v>
+        <v>17.1491512979098</v>
       </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="3">
-        <v>45575</v>
+      <c r="A29" s="4">
+        <v>45425</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C29" t="s">
         <v>47</v>
       </c>
       <c r="D29" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E29" s="2">
-        <v>12.254949928414266</v>
+        <v>6.1133684042290115</v>
       </c>
       <c r="F29">
         <v>1</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="3">
-        <v>45647</v>
+        <v>45440</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C30" t="s">
         <v>47</v>
       </c>
       <c r="D30" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E30" s="2">
-        <v>5.0872433310860332</v>
+        <v>123.23149154686199</v>
       </c>
       <c r="F30">
         <v>1</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="4">
-        <v>45321</v>
+        <v>45440</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="C31" t="s">
         <v>47</v>
       </c>
       <c r="D31" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E31" s="2">
-        <v>66.682283323879389</v>
+        <v>17.678550959111202</v>
       </c>
       <c r="F31">
         <v>1</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="3">
-        <v>45412</v>
+        <v>45441</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C32" t="s">
         <v>47</v>
       </c>
       <c r="D32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E32" s="2">
-        <v>29.286465301629605</v>
+        <v>8.1161906117480633</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32">
         <v>1</v>
@@ -1529,53 +1397,53 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="4">
-        <v>45481</v>
+        <v>45442</v>
       </c>
       <c r="B33" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="C33" t="s">
         <v>47</v>
       </c>
       <c r="D33" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E33" s="2">
-        <v>10.705744648820099</v>
+        <v>27.674824235526113</v>
       </c>
       <c r="F33">
         <v>1</v>
       </c>
       <c r="G33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="3">
-        <v>45311</v>
+        <v>45447</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C34" t="s">
         <v>47</v>
       </c>
       <c r="D34" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E34" s="2">
-        <v>50.089501984960542</v>
+        <v>21.17005254480171</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="3">
-        <v>45503</v>
+      <c r="A35" s="4">
+        <v>45450</v>
       </c>
       <c r="B35" t="s">
         <v>23</v>
@@ -1587,7 +1455,7 @@
         <v>10</v>
       </c>
       <c r="E35" s="2">
-        <v>387.46481586504211</v>
+        <v>182.33130768296445</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -1598,33 +1466,33 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="3">
-        <v>45561</v>
+        <v>45451</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C36" t="s">
         <v>47</v>
       </c>
       <c r="D36" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E36" s="2">
-        <v>65.067093202924426</v>
+        <v>15.374193649330747</v>
       </c>
       <c r="F36">
         <v>1</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="3">
-        <v>45642</v>
+      <c r="A37" s="4">
+        <v>45454</v>
       </c>
       <c r="B37" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C37" t="s">
         <v>47</v>
@@ -1633,7 +1501,7 @@
         <v>10</v>
       </c>
       <c r="E37" s="2">
-        <v>207.00141369968208</v>
+        <v>17.586058947264888</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -1644,68 +1512,68 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="3">
-        <v>45423</v>
+        <v>45456</v>
       </c>
       <c r="B38" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C38" t="s">
         <v>47</v>
       </c>
       <c r="D38" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E38" s="2">
-        <v>17.1491512979098</v>
+        <v>11.907243878342793</v>
       </c>
       <c r="F38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="3">
-        <v>45623</v>
+      <c r="A39" s="4">
+        <v>45457</v>
       </c>
       <c r="B39" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C39" t="s">
         <v>47</v>
       </c>
       <c r="D39" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E39" s="2">
-        <v>18.750558620364448</v>
+        <v>9.0713740385982007</v>
       </c>
       <c r="F39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G39">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="3">
-        <v>45527</v>
+        <v>45458</v>
       </c>
       <c r="B40" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C40" t="s">
         <v>47</v>
       </c>
       <c r="D40" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E40" s="2">
-        <v>100.18836650895901</v>
+        <v>4.4450988443080242</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40">
         <v>1</v>
@@ -1713,22 +1581,22 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="4">
-        <v>45311</v>
+        <v>45462</v>
       </c>
       <c r="B41" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C41" t="s">
         <v>47</v>
       </c>
       <c r="D41" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E41" s="2">
-        <v>23.170220279194677</v>
+        <v>6.1362243634941409</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41">
         <v>1</v>
@@ -1736,88 +1604,88 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="3">
-        <v>45486</v>
+        <v>45468</v>
       </c>
       <c r="B42" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="C42" t="s">
         <v>47</v>
       </c>
       <c r="D42" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E42" s="2">
-        <v>28.990897890685307</v>
+        <v>26.169127192058014</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="4">
-        <v>45562</v>
+        <v>45470</v>
       </c>
       <c r="B43" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="C43" t="s">
         <v>47</v>
       </c>
       <c r="D43" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E43" s="2">
-        <v>16.830074653529735</v>
+        <v>184.65116515446616</v>
       </c>
       <c r="F43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="4">
-        <v>45542</v>
+      <c r="A44" s="3">
+        <v>45472</v>
       </c>
       <c r="B44" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C44" t="s">
         <v>47</v>
       </c>
       <c r="D44" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="2">
+        <v>45.904357736606926</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="4">
+        <v>45474</v>
+      </c>
+      <c r="B45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="2">
-        <v>21.577894032917253</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="3">
-        <v>45456</v>
-      </c>
-      <c r="B45" t="s">
-        <v>35</v>
-      </c>
-      <c r="C45" t="s">
-        <v>47</v>
-      </c>
-      <c r="D45" t="s">
-        <v>17</v>
-      </c>
       <c r="E45" s="2">
-        <v>11.907243878342793</v>
+        <v>32.529640875787123</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -1827,23 +1695,23 @@
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="4">
-        <v>45543</v>
+      <c r="A46" s="3">
+        <v>45478</v>
       </c>
       <c r="B46" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C46" t="s">
         <v>47</v>
       </c>
       <c r="D46" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E46" s="2">
-        <v>25.003529250849283</v>
+        <v>16.073972115983096</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46">
         <v>1</v>
@@ -1851,76 +1719,76 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="4">
-        <v>45450</v>
+        <v>45481</v>
       </c>
       <c r="B47" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C47" t="s">
         <v>47</v>
       </c>
       <c r="D47" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E47" s="2">
-        <v>182.33130768296445</v>
+        <v>10.705744648820099</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="3">
-        <v>45440</v>
+        <v>45486</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="C48" t="s">
         <v>47</v>
       </c>
       <c r="D48" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E48" s="2">
-        <v>123.23149154686199</v>
+        <v>28.990897890685307</v>
       </c>
       <c r="F48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G48">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="4">
-        <v>45379</v>
+        <v>45494</v>
       </c>
       <c r="B49" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C49" t="s">
         <v>47</v>
       </c>
       <c r="D49" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E49" s="2">
-        <v>91.115032457869006</v>
+        <v>126.59078627224213</v>
       </c>
       <c r="F49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="3">
-        <v>45368</v>
+        <v>45495</v>
       </c>
       <c r="B50" t="s">
         <v>8</v>
@@ -1932,7 +1800,7 @@
         <v>8</v>
       </c>
       <c r="E50" s="2">
-        <v>34.412227678898994</v>
+        <v>12.061717676004944</v>
       </c>
       <c r="F50">
         <v>1</v>
@@ -1943,56 +1811,56 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="4">
-        <v>45323</v>
+        <v>45499</v>
       </c>
       <c r="B51" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C51" t="s">
         <v>47</v>
       </c>
       <c r="D51" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E51" s="2">
-        <v>23.859230634878017</v>
+        <v>4.0793809055140491</v>
       </c>
       <c r="F51">
         <v>1</v>
       </c>
       <c r="G51">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="4">
-        <v>45353</v>
+      <c r="A52" s="3">
+        <v>45503</v>
       </c>
       <c r="B52" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C52" t="s">
         <v>47</v>
       </c>
       <c r="D52" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E52" s="2">
-        <v>8.4678212748500812</v>
+        <v>387.46481586504211</v>
       </c>
       <c r="F52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G52">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="3">
-        <v>45332</v>
+      <c r="A53" s="4">
+        <v>45510</v>
       </c>
       <c r="B53" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C53" t="s">
         <v>47</v>
@@ -2001,7 +1869,7 @@
         <v>16</v>
       </c>
       <c r="E53" s="2">
-        <v>24.677305430093984</v>
+        <v>3.8086864651546297</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -2011,8 +1879,8 @@
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="4">
-        <v>45575</v>
+      <c r="A54" s="3">
+        <v>45514</v>
       </c>
       <c r="B54" t="s">
         <v>12</v>
@@ -2024,7 +1892,7 @@
         <v>11</v>
       </c>
       <c r="E54" s="2">
-        <v>43.357284027160432</v>
+        <v>47.202743940079138</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -2035,30 +1903,30 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="4">
-        <v>45577</v>
+        <v>45515</v>
       </c>
       <c r="B55" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="C55" t="s">
         <v>47</v>
       </c>
       <c r="D55" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E55" s="2">
-        <v>24.960541772205787</v>
+        <v>45.542571114625908</v>
       </c>
       <c r="F55">
         <v>1</v>
       </c>
       <c r="G55">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="3">
-        <v>45578</v>
+        <v>45521</v>
       </c>
       <c r="B56" t="s">
         <v>8</v>
@@ -2070,7 +1938,7 @@
         <v>8</v>
       </c>
       <c r="E56" s="2">
-        <v>29.512426669497486</v>
+        <v>29.018191431636822</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -2080,69 +1948,69 @@
       </c>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="3">
-        <v>45402</v>
+      <c r="A57" s="4">
+        <v>45524</v>
       </c>
       <c r="B57" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="C57" t="s">
         <v>47</v>
       </c>
       <c r="D57" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E57" s="2">
-        <v>138.2147422166174</v>
+        <v>8.9102359077551156</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:7">
-      <c r="A58" s="4">
-        <v>45442</v>
+      <c r="A58" s="3">
+        <v>45527</v>
       </c>
       <c r="B58" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C58" t="s">
         <v>47</v>
       </c>
       <c r="D58" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E58" s="2">
-        <v>27.674824235526113</v>
+        <v>100.18836650895901</v>
       </c>
       <c r="F58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G58">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="4">
-        <v>45419</v>
+        <v>45528</v>
       </c>
       <c r="B59" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="C59" t="s">
         <v>47</v>
       </c>
       <c r="D59" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E59" s="2">
-        <v>25.568377219304327</v>
+        <v>39.268263806949975</v>
       </c>
       <c r="F59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -2150,22 +2018,22 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="3">
-        <v>45629</v>
+        <v>45536</v>
       </c>
       <c r="B60" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="C60" t="s">
         <v>47</v>
       </c>
       <c r="D60" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E60" s="2">
-        <v>10.924223157404425</v>
+        <v>13.768101260551122</v>
       </c>
       <c r="F60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G60">
         <v>1</v>
@@ -2173,33 +2041,33 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="4">
-        <v>45528</v>
+        <v>45540</v>
       </c>
       <c r="B61" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C61" t="s">
         <v>47</v>
       </c>
       <c r="D61" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E61" s="2">
-        <v>39.268263806949975</v>
+        <v>10.843589715267399</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G61">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="3">
-        <v>45536</v>
+        <v>45541</v>
       </c>
       <c r="B62" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C62" t="s">
         <v>47</v>
@@ -2208,7 +2076,7 @@
         <v>16</v>
       </c>
       <c r="E62" s="2">
-        <v>13.768101260551122</v>
+        <v>9.5459497283993091</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -2219,42 +2087,42 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="4">
-        <v>45393</v>
+        <v>45542</v>
       </c>
       <c r="B63" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C63" t="s">
         <v>47</v>
       </c>
       <c r="D63" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E63" s="2">
-        <v>3.6981094178656995</v>
+        <v>21.577894032917253</v>
       </c>
       <c r="F63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G63">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="4">
-        <v>45647</v>
+      <c r="A64" s="3">
+        <v>45543</v>
       </c>
       <c r="B64" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C64" t="s">
         <v>47</v>
       </c>
       <c r="D64" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E64" s="2">
-        <v>11.866231020207174</v>
+        <v>8.218023793872284</v>
       </c>
       <c r="F64">
         <v>0</v>
@@ -2264,11 +2132,11 @@
       </c>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65" s="3">
-        <v>45441</v>
+      <c r="A65" s="4">
+        <v>45543</v>
       </c>
       <c r="B65" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C65" t="s">
         <v>47</v>
@@ -2277,7 +2145,7 @@
         <v>16</v>
       </c>
       <c r="E65" s="2">
-        <v>8.1161906117480633</v>
+        <v>25.003529250849283</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -2288,22 +2156,22 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="3">
-        <v>45639</v>
+        <v>45547</v>
       </c>
       <c r="B66" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C66" t="s">
         <v>47</v>
       </c>
       <c r="D66" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E66" s="2">
-        <v>8.8561344087601057</v>
+        <v>19.033404509807344</v>
       </c>
       <c r="F66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G66">
         <v>1</v>
@@ -2311,68 +2179,68 @@
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="4">
-        <v>45406</v>
+        <v>45552</v>
       </c>
       <c r="B67" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C67" t="s">
         <v>47</v>
       </c>
       <c r="D67" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E67" s="2">
-        <v>59.465543593581948</v>
+        <v>45.124918956005892</v>
       </c>
       <c r="F67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G67">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="4">
-        <v>45639</v>
+      <c r="A68" s="3">
+        <v>45561</v>
       </c>
       <c r="B68" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C68" t="s">
         <v>47</v>
       </c>
       <c r="D68" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E68" s="2">
-        <v>26.00967141893349</v>
+        <v>65.067093202924426</v>
       </c>
       <c r="F68">
         <v>1</v>
       </c>
       <c r="G68">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" s="4">
-        <v>45494</v>
+        <v>45562</v>
       </c>
       <c r="B69" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="C69" t="s">
         <v>47</v>
       </c>
       <c r="D69" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E69" s="2">
-        <v>126.59078627224213</v>
+        <v>16.830074653529735</v>
       </c>
       <c r="F69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G69">
         <v>1</v>
@@ -2380,206 +2248,206 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="3">
-        <v>45317</v>
+        <v>45572</v>
       </c>
       <c r="B70" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C70" t="s">
         <v>47</v>
       </c>
       <c r="D70" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E70" s="2">
-        <v>546.34269896948445</v>
+        <v>18.005409657329089</v>
       </c>
       <c r="F70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G70">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:7">
-      <c r="A71" s="4">
-        <v>45510</v>
+      <c r="A71" s="3">
+        <v>45575</v>
       </c>
       <c r="B71" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C71" t="s">
         <v>47</v>
       </c>
       <c r="D71" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E71" s="2">
-        <v>3.8086864651546297</v>
+        <v>12.254949928414266</v>
       </c>
       <c r="F71">
         <v>1</v>
       </c>
       <c r="G71">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="4">
-        <v>45524</v>
+        <v>45575</v>
       </c>
       <c r="B72" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C72" t="s">
         <v>47</v>
       </c>
       <c r="D72" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E72" s="2">
-        <v>8.9102359077551156</v>
+        <v>43.357284027160432</v>
       </c>
       <c r="F72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G72">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="4">
-        <v>45440</v>
+        <v>45577</v>
       </c>
       <c r="B73" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="C73" t="s">
         <v>47</v>
       </c>
       <c r="D73" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E73" s="2">
-        <v>17.678550959111202</v>
+        <v>24.960541772205787</v>
       </c>
       <c r="F73">
         <v>1</v>
       </c>
       <c r="G73">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:7">
-      <c r="A74" s="4">
-        <v>45622</v>
+      <c r="A74" s="3">
+        <v>45578</v>
       </c>
       <c r="B74" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C74" t="s">
         <v>47</v>
       </c>
       <c r="D74" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E74" s="2">
-        <v>4.0966721465376077</v>
+        <v>29.512426669497486</v>
       </c>
       <c r="F74">
         <v>1</v>
       </c>
       <c r="G74">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" s="4">
-        <v>45628</v>
+        <v>45582</v>
       </c>
       <c r="B75" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C75" t="s">
         <v>47</v>
       </c>
       <c r="D75" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E75" s="2">
-        <v>5.4404930268114597</v>
+        <v>17.80165241729523</v>
       </c>
       <c r="F75">
         <v>1</v>
       </c>
       <c r="G75">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:7">
-      <c r="A76" s="4">
-        <v>45315</v>
+      <c r="A76" s="3">
+        <v>45593</v>
       </c>
       <c r="B76" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="C76" t="s">
         <v>47</v>
       </c>
       <c r="D76" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E76" s="2">
-        <v>18.209604367663978</v>
+        <v>47.674742913663458</v>
       </c>
       <c r="F76">
         <v>0</v>
       </c>
       <c r="G76">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:7">
-      <c r="A77" s="3">
-        <v>45472</v>
+      <c r="A77" s="4">
+        <v>45594</v>
       </c>
       <c r="B77" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C77" t="s">
         <v>47</v>
       </c>
       <c r="D77" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" s="2">
+        <v>53.524381510800161</v>
+      </c>
+      <c r="F77">
+        <v>1</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="3">
+        <v>45595</v>
+      </c>
+      <c r="B78" t="s">
+        <v>18</v>
+      </c>
+      <c r="C78" t="s">
+        <v>47</v>
+      </c>
+      <c r="D78" t="s">
         <v>11</v>
       </c>
-      <c r="E77" s="2">
-        <v>45.904357736606926</v>
-      </c>
-      <c r="F77">
-        <v>0</v>
-      </c>
-      <c r="G77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
-      <c r="A78" s="4">
-        <v>45396</v>
-      </c>
-      <c r="B78" t="s">
-        <v>8</v>
-      </c>
-      <c r="C78" t="s">
-        <v>47</v>
-      </c>
-      <c r="D78" t="s">
-        <v>8</v>
-      </c>
       <c r="E78" s="2">
-        <v>60.015682920995474</v>
+        <v>6.8664125929764026</v>
       </c>
       <c r="F78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -2587,19 +2455,19 @@
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="4">
-        <v>45454</v>
+        <v>45595</v>
       </c>
       <c r="B79" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="C79" t="s">
         <v>47</v>
       </c>
       <c r="D79" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E79" s="2">
-        <v>17.586058947264888</v>
+        <v>20.148806473862361</v>
       </c>
       <c r="F79">
         <v>0</v>
@@ -2609,66 +2477,66 @@
       </c>
     </row>
     <row r="80" spans="1:7">
-      <c r="A80" s="4">
-        <v>45582</v>
+      <c r="A80" s="3">
+        <v>45610</v>
       </c>
       <c r="B80" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C80" t="s">
         <v>47</v>
       </c>
       <c r="D80" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E80" s="2">
-        <v>17.80165241729523</v>
+        <v>23.409850623813977</v>
       </c>
       <c r="F80">
         <v>1</v>
       </c>
       <c r="G80">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" s="4">
-        <v>45594</v>
+        <v>45622</v>
       </c>
       <c r="B81" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C81" t="s">
         <v>47</v>
       </c>
       <c r="D81" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E81" s="2">
-        <v>53.524381510800161</v>
+        <v>4.0966721465376077</v>
       </c>
       <c r="F81">
         <v>1</v>
       </c>
       <c r="G81">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:7">
-      <c r="A82" s="4">
-        <v>45425</v>
+      <c r="A82" s="3">
+        <v>45623</v>
       </c>
       <c r="B82" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C82" t="s">
         <v>47</v>
       </c>
       <c r="D82" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E82" s="2">
-        <v>6.1133684042290115</v>
+        <v>18.750558620364448</v>
       </c>
       <c r="F82">
         <v>1</v>
@@ -2679,42 +2547,42 @@
     </row>
     <row r="83" spans="1:7">
       <c r="A83" s="3">
-        <v>45541</v>
+        <v>45627</v>
       </c>
       <c r="B83" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C83" t="s">
         <v>47</v>
       </c>
       <c r="D83" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E83" s="2">
-        <v>9.5459497283993091</v>
+        <v>55.806989867356052</v>
       </c>
       <c r="F83">
         <v>1</v>
       </c>
       <c r="G83">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:7">
-      <c r="A84" s="3">
-        <v>45644</v>
+      <c r="A84" s="4">
+        <v>45627</v>
       </c>
       <c r="B84" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="C84" t="s">
         <v>47</v>
       </c>
       <c r="D84" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E84" s="2">
-        <v>28.282964012150725</v>
+        <v>38.079442340158884</v>
       </c>
       <c r="F84">
         <v>0</v>
@@ -2725,7 +2593,7 @@
     </row>
     <row r="85" spans="1:7">
       <c r="A85" s="4">
-        <v>45499</v>
+        <v>45628</v>
       </c>
       <c r="B85" t="s">
         <v>27</v>
@@ -2737,7 +2605,7 @@
         <v>16</v>
       </c>
       <c r="E85" s="2">
-        <v>4.0793809055140491</v>
+        <v>5.4404930268114597</v>
       </c>
       <c r="F85">
         <v>1</v>
@@ -2748,33 +2616,33 @@
     </row>
     <row r="86" spans="1:7">
       <c r="A86" s="3">
-        <v>45521</v>
+        <v>45629</v>
       </c>
       <c r="B86" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="C86" t="s">
         <v>47</v>
       </c>
       <c r="D86" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E86" s="2">
-        <v>29.018191431636822</v>
+        <v>10.924223157404425</v>
       </c>
       <c r="F86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G86">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" s="4">
-        <v>45595</v>
+        <v>45632</v>
       </c>
       <c r="B87" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="C87" t="s">
         <v>47</v>
@@ -2783,99 +2651,99 @@
         <v>7</v>
       </c>
       <c r="E87" s="2">
-        <v>20.148806473862361</v>
+        <v>33.706145994917662</v>
       </c>
       <c r="F87">
         <v>0</v>
       </c>
       <c r="G87">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" s="3">
-        <v>45495</v>
+        <v>45639</v>
       </c>
       <c r="B88" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C88" t="s">
         <v>47</v>
       </c>
       <c r="D88" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E88" s="2">
-        <v>12.061717676004944</v>
+        <v>8.8561344087601057</v>
       </c>
       <c r="F88">
         <v>1</v>
       </c>
       <c r="G88">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:7">
-      <c r="A89" s="3">
-        <v>45468</v>
+      <c r="A89" s="4">
+        <v>45639</v>
       </c>
       <c r="B89" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C89" t="s">
         <v>47</v>
       </c>
       <c r="D89" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E89" s="2">
-        <v>26.169127192058014</v>
+        <v>26.00967141893349</v>
       </c>
       <c r="F89">
         <v>1</v>
       </c>
       <c r="G89">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" s="4">
-        <v>45336</v>
+        <v>45642</v>
       </c>
       <c r="B90" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C90" t="s">
         <v>47</v>
       </c>
       <c r="D90" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E90" s="2">
-        <v>4.1295821605673417</v>
+        <v>35.881275421039959</v>
       </c>
       <c r="F90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G90">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:7">
-      <c r="A91" s="4">
-        <v>45627</v>
+      <c r="A91" s="3">
+        <v>45642</v>
       </c>
       <c r="B91" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C91" t="s">
         <v>47</v>
       </c>
       <c r="D91" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E91" s="2">
-        <v>38.079442340158884</v>
+        <v>207.00141369968208</v>
       </c>
       <c r="F91">
         <v>0</v>
@@ -2886,10 +2754,10 @@
     </row>
     <row r="92" spans="1:7">
       <c r="A92" s="3">
-        <v>45380</v>
+        <v>45644</v>
       </c>
       <c r="B92" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C92" t="s">
         <v>47</v>
@@ -2898,7 +2766,7 @@
         <v>17</v>
       </c>
       <c r="E92" s="2">
-        <v>61.350532464411664</v>
+        <v>28.282964012150725</v>
       </c>
       <c r="F92">
         <v>0</v>
@@ -2909,10 +2777,10 @@
     </row>
     <row r="93" spans="1:7">
       <c r="A93" s="3">
-        <v>45610</v>
+        <v>45647</v>
       </c>
       <c r="B93" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C93" t="s">
         <v>47</v>
@@ -2921,7 +2789,7 @@
         <v>16</v>
       </c>
       <c r="E93" s="2">
-        <v>23.409850623813977</v>
+        <v>5.0872433310860332</v>
       </c>
       <c r="F93">
         <v>1</v>
@@ -2932,19 +2800,19 @@
     </row>
     <row r="94" spans="1:7">
       <c r="A94" s="4">
-        <v>45470</v>
+        <v>45647</v>
       </c>
       <c r="B94" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C94" t="s">
         <v>47</v>
       </c>
       <c r="D94" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E94" s="2">
-        <v>184.65116515446616</v>
+        <v>11.866231020207174</v>
       </c>
       <c r="F94">
         <v>0</v>
@@ -2955,10 +2823,10 @@
     </row>
     <row r="95" spans="1:7">
       <c r="A95" s="5">
-        <v>45451</v>
+        <v>45653</v>
       </c>
       <c r="B95" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C95" t="s">
         <v>47</v>
@@ -2967,7 +2835,7 @@
         <v>16</v>
       </c>
       <c r="E95" s="2">
-        <v>15.374193649330747</v>
+        <v>4.5444022945078419</v>
       </c>
       <c r="F95">
         <v>1</v>
@@ -2983,880 +2851,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3EB3251-4FC4-4EFB-A336-AF1B21393CF0}">
-  <dimension ref="A1:B95"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A95" sqref="A2:A95"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="9.140625" style="6"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3">
-        <v>45392</v>
-      </c>
-      <c r="B2" s="7">
-        <f ca="1">RAND()</f>
-        <v>0.85578244643325097</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="4">
-        <v>45389</v>
-      </c>
-      <c r="B3" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.25868480386181769</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3">
-        <v>45595</v>
-      </c>
-      <c r="B4" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.95256536777368939</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="3">
-        <v>45394</v>
-      </c>
-      <c r="B5" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.24570250096690072</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="4">
-        <v>45474</v>
-      </c>
-      <c r="B6" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.88926977601240798</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="3">
-        <v>45547</v>
-      </c>
-      <c r="B7" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.50973328972371734</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="4">
-        <v>45515</v>
-      </c>
-      <c r="B8" s="8">
-        <f ca="1">RAND()</f>
-        <v>8.7152480175947011E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="3">
-        <v>45395</v>
-      </c>
-      <c r="B9" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.83048609417028951</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="3">
-        <v>45322</v>
-      </c>
-      <c r="B10" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.61070733637547781</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="4">
-        <v>45642</v>
-      </c>
-      <c r="B11" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.38439401418439734</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="3">
-        <v>45478</v>
-      </c>
-      <c r="B12" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.71555605598590732</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="4">
-        <v>45395</v>
-      </c>
-      <c r="B13" s="8">
-        <f ca="1">RAND()</f>
-        <v>2.8660435720706423E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="4">
-        <v>45632</v>
-      </c>
-      <c r="B14" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.34920150066905342</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="4">
-        <v>45552</v>
-      </c>
-      <c r="B15" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.89805961479960439</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="3">
-        <v>45447</v>
-      </c>
-      <c r="B16" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.10632000241014761</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="4">
-        <v>45462</v>
-      </c>
-      <c r="B17" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.34985961417205869</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="4">
-        <v>45457</v>
-      </c>
-      <c r="B18" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.87909017080111329</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="3">
-        <v>45543</v>
-      </c>
-      <c r="B19" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.12682576385696909</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="3">
-        <v>45627</v>
-      </c>
-      <c r="B20" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.70161418122212371</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="3">
-        <v>45458</v>
-      </c>
-      <c r="B21" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.174092124976995</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="4">
-        <v>45540</v>
-      </c>
-      <c r="B22" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.85813713515690637</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="4">
-        <v>45653</v>
-      </c>
-      <c r="B23" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.92769661309063245</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="3">
-        <v>45514</v>
-      </c>
-      <c r="B24" s="8">
-        <f ca="1">RAND()</f>
-        <v>4.0457960526361192E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="3">
-        <v>45572</v>
-      </c>
-      <c r="B25" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.23119809439957317</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="3">
-        <v>45593</v>
-      </c>
-      <c r="B26" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.87364343202114336</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="3">
-        <v>45292</v>
-      </c>
-      <c r="B27" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.19930195534507456</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="3">
-        <v>45350</v>
-      </c>
-      <c r="B28" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.56908938877260018</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="3">
-        <v>45575</v>
-      </c>
-      <c r="B29" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.1834918878078533</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="3">
-        <v>45647</v>
-      </c>
-      <c r="B30" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.70276410732441319</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="4">
-        <v>45321</v>
-      </c>
-      <c r="B31" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.96973680072099011</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="3">
-        <v>45412</v>
-      </c>
-      <c r="B32" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.95695223136207519</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="4">
-        <v>45481</v>
-      </c>
-      <c r="B33" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.54494772659994861</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="3">
-        <v>45311</v>
-      </c>
-      <c r="B34" s="8">
-        <f ca="1">RAND()</f>
-        <v>8.5560096793153129E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="3">
-        <v>45503</v>
-      </c>
-      <c r="B35" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.6703306554177173</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="3">
-        <v>45561</v>
-      </c>
-      <c r="B36" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.82062941447455451</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="3">
-        <v>45642</v>
-      </c>
-      <c r="B37" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.8994579326794484</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="3">
-        <v>45423</v>
-      </c>
-      <c r="B38" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.62126540421724996</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="3">
-        <v>45623</v>
-      </c>
-      <c r="B39" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.28488955844280095</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="3">
-        <v>45527</v>
-      </c>
-      <c r="B40" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.77063095355079647</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="4">
-        <v>45311</v>
-      </c>
-      <c r="B41" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.23843633567143829</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="3">
-        <v>45486</v>
-      </c>
-      <c r="B42" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.15151387091237511</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="4">
-        <v>45562</v>
-      </c>
-      <c r="B43" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.94757273221392191</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="4">
-        <v>45542</v>
-      </c>
-      <c r="B44" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.57745097621284802</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="3">
-        <v>45456</v>
-      </c>
-      <c r="B45" s="8">
-        <f ca="1">RAND()</f>
-        <v>8.7774973824360725E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="4">
-        <v>45543</v>
-      </c>
-      <c r="B46" s="8">
-        <f ca="1">RAND()</f>
-        <v>8.8492998499789532E-3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="4">
-        <v>45450</v>
-      </c>
-      <c r="B47" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.25106612858976918</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="3">
-        <v>45440</v>
-      </c>
-      <c r="B48" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.92494608066473916</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="4">
-        <v>45379</v>
-      </c>
-      <c r="B49" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.13128715402125635</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="3">
-        <v>45368</v>
-      </c>
-      <c r="B50" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.9497266291189328</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="4">
-        <v>45323</v>
-      </c>
-      <c r="B51" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.89071685052303606</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="4">
-        <v>45353</v>
-      </c>
-      <c r="B52" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.71101741223270487</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="3">
-        <v>45332</v>
-      </c>
-      <c r="B53" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.30231207521674508</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="4">
-        <v>45575</v>
-      </c>
-      <c r="B54" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.16149597519477776</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="4">
-        <v>45577</v>
-      </c>
-      <c r="B55" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.10640268008457532</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="3">
-        <v>45578</v>
-      </c>
-      <c r="B56" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.34347492239365274</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="3">
-        <v>45402</v>
-      </c>
-      <c r="B57" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.1794364947339615</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="4">
-        <v>45442</v>
-      </c>
-      <c r="B58" s="8">
-        <f ca="1">RAND()</f>
-        <v>2.4024314216216092E-2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="4">
-        <v>45419</v>
-      </c>
-      <c r="B59" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.85943760866372065</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="3">
-        <v>45629</v>
-      </c>
-      <c r="B60" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.28042400160368075</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="4">
-        <v>45528</v>
-      </c>
-      <c r="B61" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.56636287417276066</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="3">
-        <v>45536</v>
-      </c>
-      <c r="B62" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.88044987314061718</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="4">
-        <v>45393</v>
-      </c>
-      <c r="B63" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.965979958880545</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="4">
-        <v>45647</v>
-      </c>
-      <c r="B64" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.96629138372225054</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="3">
-        <v>45441</v>
-      </c>
-      <c r="B65" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.35208131214473026</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="3">
-        <v>45639</v>
-      </c>
-      <c r="B66" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.34938823880436753</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="4">
-        <v>45406</v>
-      </c>
-      <c r="B67" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.66599102966258428</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="4">
-        <v>45639</v>
-      </c>
-      <c r="B68" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.36825600756529508</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="4">
-        <v>45494</v>
-      </c>
-      <c r="B69" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.99138484261872206</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="3">
-        <v>45317</v>
-      </c>
-      <c r="B70" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.47113421614946283</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="4">
-        <v>45510</v>
-      </c>
-      <c r="B71" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.24726097858480323</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="4">
-        <v>45524</v>
-      </c>
-      <c r="B72" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.64352932889279424</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="4">
-        <v>45440</v>
-      </c>
-      <c r="B73" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.79308458863630349</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="4">
-        <v>45622</v>
-      </c>
-      <c r="B74" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.40311941701152443</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="4">
-        <v>45628</v>
-      </c>
-      <c r="B75" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.39053456248145868</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="4">
-        <v>45315</v>
-      </c>
-      <c r="B76" s="8">
-        <f ca="1">RAND()</f>
-        <v>4.6156534315552666E-2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="3">
-        <v>45472</v>
-      </c>
-      <c r="B77" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.77887780156762576</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="4">
-        <v>45396</v>
-      </c>
-      <c r="B78" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.57634000273619357</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="4">
-        <v>45454</v>
-      </c>
-      <c r="B79" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.58542217707576805</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="A80" s="4">
-        <v>45582</v>
-      </c>
-      <c r="B80" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.68824709944652485</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="4">
-        <v>45594</v>
-      </c>
-      <c r="B81" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.18753799905952051</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="4">
-        <v>45425</v>
-      </c>
-      <c r="B82" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.40411463989093455</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="3">
-        <v>45541</v>
-      </c>
-      <c r="B83" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.65503260925826423</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="3">
-        <v>45644</v>
-      </c>
-      <c r="B84" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.23173286309322583</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="4">
-        <v>45499</v>
-      </c>
-      <c r="B85" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.67741797697289896</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="3">
-        <v>45521</v>
-      </c>
-      <c r="B86" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.85323660787144751</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="4">
-        <v>45595</v>
-      </c>
-      <c r="B87" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.3188585614040218</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="A88" s="3">
-        <v>45495</v>
-      </c>
-      <c r="B88" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.80843259148070079</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="3">
-        <v>45468</v>
-      </c>
-      <c r="B89" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.72494968688368633</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="4">
-        <v>45336</v>
-      </c>
-      <c r="B90" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.44626805547395232</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="4">
-        <v>45627</v>
-      </c>
-      <c r="B91" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.17731858176842152</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="3">
-        <v>45380</v>
-      </c>
-      <c r="B92" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.39533969461135743</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="3">
-        <v>45610</v>
-      </c>
-      <c r="B93" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.628708744239313</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" s="4">
-        <v>45470</v>
-      </c>
-      <c r="B94" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.46037730855780323</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" s="5">
-        <v>45451</v>
-      </c>
-      <c r="B95" s="9">
-        <f ca="1">RAND()</f>
-        <v>0.39623598571142937</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
clean up sample data (#34)
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Documents\Stuff\Logic\Coding Projects\lisser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CAF1946-B2BD-458F-903E-E81D6C721078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421770A4-8F15-4E33-AA27-E2E7E9FC6999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -178,9 +177,6 @@
   </si>
   <si>
     <t>_redacted_</t>
-  </si>
-  <si>
-    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -191,7 +187,7 @@
     <numFmt numFmtId="164" formatCode="m/d;@"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,12 +199,6 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -225,7 +215,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -251,17 +241,6 @@
         <color theme="1"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right/>
       <top style="thin">
         <color theme="1"/>
       </top>
@@ -275,23 +254,22 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="m/d;@"/>
       <fill>
@@ -315,100 +293,6 @@
         <horizontal/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -429,31 +313,15 @@
     <sortCondition ref="A1:A95"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Description"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Vendor"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Category"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Price" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Price" dataDxfId="0"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Is Food"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Controllable"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A911DC3C-FA4C-4527-9662-3E2BD75E264A}" name="Table3" displayName="Table3" ref="A1:B95" totalsRowShown="0" dataDxfId="2" tableBorderDxfId="4">
-  <autoFilter ref="A1:B95" xr:uid="{A911DC3C-FA4C-4527-9662-3E2BD75E264A}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B95">
-    <sortCondition ref="B1:B95"/>
-  </sortState>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{AC37F961-34F0-45E8-B984-00213DE133FC}" name="Date" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{6FCA42A8-F454-4965-8DB0-37B5B16651F9}" name="Column1" dataDxfId="1">
-      <calculatedColumnFormula>RAND()</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -776,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A95" sqref="A2:A95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -816,88 +684,88 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3">
-        <v>45392</v>
+        <v>45292</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E2" s="2">
-        <v>51.03421481904099</v>
+        <v>17.147002791824256</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="4">
-        <v>45389</v>
+      <c r="A3" s="3">
+        <v>45311</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>21.525176317465011</v>
+        <v>50.089501984960542</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="3">
-        <v>45595</v>
+      <c r="A4" s="4">
+        <v>45311</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
         <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2">
-        <v>6.8664125929764026</v>
+        <v>23.170220279194677</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="3">
-        <v>45394</v>
+      <c r="A5" s="4">
+        <v>45315</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
         <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2">
-        <v>52.128344351505071</v>
+        <v>18.209604367663978</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -907,11 +775,11 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="4">
-        <v>45474</v>
+      <c r="A6" s="3">
+        <v>45317</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
         <v>47</v>
@@ -920,7 +788,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="2">
-        <v>32.529640875787123</v>
+        <v>546.34269896948445</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -930,31 +798,31 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="3">
-        <v>45547</v>
+      <c r="A7" s="4">
+        <v>45321</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
         <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E7" s="2">
-        <v>19.033404509807344</v>
+        <v>66.682283323879389</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="4">
-        <v>45515</v>
+      <c r="A8" s="3">
+        <v>45322</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -966,7 +834,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>45.542571114625908</v>
+        <v>9.7536737962057725</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -976,100 +844,100 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="3">
-        <v>45395</v>
+      <c r="A9" s="4">
+        <v>45323</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
         <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2">
-        <v>18.449348228187279</v>
+        <v>23.859230634878017</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="3">
-        <v>45322</v>
+        <v>45332</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
         <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E10" s="2">
-        <v>9.7536737962057725</v>
+        <v>24.677305430093984</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4">
-        <v>45642</v>
+        <v>45336</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
         <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E11" s="2">
-        <v>35.881275421039959</v>
+        <v>4.1295821605673417</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="3">
-        <v>45478</v>
+        <v>45350</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
         <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E12" s="2">
-        <v>16.073972115983096</v>
+        <v>67.686150075286932</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="4">
-        <v>45395</v>
+        <v>45353</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
@@ -1081,7 +949,7 @@
         <v>8</v>
       </c>
       <c r="E13" s="2">
-        <v>50.319058517747656</v>
+        <v>8.4678212748500812</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -1091,184 +959,184 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="4">
-        <v>45632</v>
+      <c r="A14" s="3">
+        <v>45368</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E14" s="2">
-        <v>33.706145994917662</v>
+        <v>34.412227678898994</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="4">
-        <v>45552</v>
+        <v>45379</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
         <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E15" s="2">
-        <v>45.124918956005892</v>
+        <v>91.115032457869006</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="3">
-        <v>45447</v>
+        <v>45380</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
         <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E16" s="2">
-        <v>21.17005254480171</v>
+        <v>61.350532464411664</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="4">
-        <v>45462</v>
+        <v>45389</v>
       </c>
       <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="2">
+        <v>21.525176317465011</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="3">
+        <v>45392</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="2">
+        <v>51.03421481904099</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="4">
+        <v>45393</v>
+      </c>
+      <c r="B19" t="s">
         <v>27</v>
       </c>
-      <c r="C17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="2">
-        <v>6.1362243634941409</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="4">
-        <v>45457</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="2">
-        <v>9.0713740385982007</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="3">
-        <v>45543</v>
-      </c>
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
       <c r="E19" s="2">
-        <v>8.218023793872284</v>
+        <v>3.6981094178656995</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="3">
-        <v>45627</v>
+        <v>45394</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
         <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E20" s="2">
-        <v>55.806989867356052</v>
+        <v>52.128344351505071</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="3">
-        <v>45458</v>
+        <v>45395</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
         <v>47</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E21" s="2">
-        <v>4.4450988443080242</v>
+        <v>18.449348228187279</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1276,56 +1144,56 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="4">
-        <v>45540</v>
+        <v>45395</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="C22" t="s">
         <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E22" s="2">
-        <v>10.843589715267399</v>
+        <v>50.319058517747656</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="4">
-        <v>45653</v>
+        <v>45396</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C23" t="s">
         <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E23" s="2">
-        <v>4.5444022945078419</v>
+        <v>60.015682920995474</v>
       </c>
       <c r="F23">
         <v>1</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="3">
-        <v>45514</v>
+        <v>45402</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
         <v>47</v>
@@ -1334,7 +1202,7 @@
         <v>11</v>
       </c>
       <c r="E24" s="2">
-        <v>47.202743940079138</v>
+        <v>138.2147422166174</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1344,184 +1212,184 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="3">
-        <v>45572</v>
+      <c r="A25" s="4">
+        <v>45406</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
         <v>47</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E25" s="2">
-        <v>18.005409657329089</v>
+        <v>59.465543593581948</v>
       </c>
       <c r="F25">
         <v>1</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="3">
-        <v>45593</v>
+        <v>45412</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C26" t="s">
         <v>47</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E26" s="2">
-        <v>47.674742913663458</v>
+        <v>29.286465301629605</v>
       </c>
       <c r="F26">
         <v>0</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="3">
-        <v>45292</v>
+      <c r="A27" s="4">
+        <v>45419</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
         <v>47</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E27" s="2">
-        <v>17.147002791824256</v>
+        <v>25.568377219304327</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="3">
-        <v>45350</v>
+        <v>45423</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
         <v>47</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E28" s="2">
-        <v>67.686150075286932</v>
+        <v>17.1491512979098</v>
       </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="3">
-        <v>45575</v>
+      <c r="A29" s="4">
+        <v>45425</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C29" t="s">
         <v>47</v>
       </c>
       <c r="D29" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E29" s="2">
-        <v>12.254949928414266</v>
+        <v>6.1133684042290115</v>
       </c>
       <c r="F29">
         <v>1</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="3">
-        <v>45647</v>
+        <v>45440</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C30" t="s">
         <v>47</v>
       </c>
       <c r="D30" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E30" s="2">
-        <v>5.0872433310860332</v>
+        <v>123.23149154686199</v>
       </c>
       <c r="F30">
         <v>1</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="4">
-        <v>45321</v>
+        <v>45440</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="C31" t="s">
         <v>47</v>
       </c>
       <c r="D31" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E31" s="2">
-        <v>66.682283323879389</v>
+        <v>17.678550959111202</v>
       </c>
       <c r="F31">
         <v>1</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="3">
-        <v>45412</v>
+        <v>45441</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C32" t="s">
         <v>47</v>
       </c>
       <c r="D32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E32" s="2">
-        <v>29.286465301629605</v>
+        <v>8.1161906117480633</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32">
         <v>1</v>
@@ -1529,53 +1397,53 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="4">
-        <v>45481</v>
+        <v>45442</v>
       </c>
       <c r="B33" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="C33" t="s">
         <v>47</v>
       </c>
       <c r="D33" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E33" s="2">
-        <v>10.705744648820099</v>
+        <v>27.674824235526113</v>
       </c>
       <c r="F33">
         <v>1</v>
       </c>
       <c r="G33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="3">
-        <v>45311</v>
+        <v>45447</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C34" t="s">
         <v>47</v>
       </c>
       <c r="D34" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E34" s="2">
-        <v>50.089501984960542</v>
+        <v>21.17005254480171</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="3">
-        <v>45503</v>
+      <c r="A35" s="4">
+        <v>45450</v>
       </c>
       <c r="B35" t="s">
         <v>23</v>
@@ -1587,7 +1455,7 @@
         <v>10</v>
       </c>
       <c r="E35" s="2">
-        <v>387.46481586504211</v>
+        <v>182.33130768296445</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -1598,33 +1466,33 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="3">
-        <v>45561</v>
+        <v>45451</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C36" t="s">
         <v>47</v>
       </c>
       <c r="D36" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E36" s="2">
-        <v>65.067093202924426</v>
+        <v>15.374193649330747</v>
       </c>
       <c r="F36">
         <v>1</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="3">
-        <v>45642</v>
+      <c r="A37" s="4">
+        <v>45454</v>
       </c>
       <c r="B37" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C37" t="s">
         <v>47</v>
@@ -1633,7 +1501,7 @@
         <v>10</v>
       </c>
       <c r="E37" s="2">
-        <v>207.00141369968208</v>
+        <v>17.586058947264888</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -1644,68 +1512,68 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="3">
-        <v>45423</v>
+        <v>45456</v>
       </c>
       <c r="B38" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C38" t="s">
         <v>47</v>
       </c>
       <c r="D38" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E38" s="2">
-        <v>17.1491512979098</v>
+        <v>11.907243878342793</v>
       </c>
       <c r="F38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="3">
-        <v>45623</v>
+      <c r="A39" s="4">
+        <v>45457</v>
       </c>
       <c r="B39" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C39" t="s">
         <v>47</v>
       </c>
       <c r="D39" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E39" s="2">
-        <v>18.750558620364448</v>
+        <v>9.0713740385982007</v>
       </c>
       <c r="F39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G39">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="3">
-        <v>45527</v>
+        <v>45458</v>
       </c>
       <c r="B40" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C40" t="s">
         <v>47</v>
       </c>
       <c r="D40" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E40" s="2">
-        <v>100.18836650895901</v>
+        <v>4.4450988443080242</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40">
         <v>1</v>
@@ -1713,22 +1581,22 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="4">
-        <v>45311</v>
+        <v>45462</v>
       </c>
       <c r="B41" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C41" t="s">
         <v>47</v>
       </c>
       <c r="D41" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E41" s="2">
-        <v>23.170220279194677</v>
+        <v>6.1362243634941409</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41">
         <v>1</v>
@@ -1736,88 +1604,88 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="3">
-        <v>45486</v>
+        <v>45468</v>
       </c>
       <c r="B42" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="C42" t="s">
         <v>47</v>
       </c>
       <c r="D42" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E42" s="2">
-        <v>28.990897890685307</v>
+        <v>26.169127192058014</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="4">
-        <v>45562</v>
+        <v>45470</v>
       </c>
       <c r="B43" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="C43" t="s">
         <v>47</v>
       </c>
       <c r="D43" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E43" s="2">
-        <v>16.830074653529735</v>
+        <v>184.65116515446616</v>
       </c>
       <c r="F43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="4">
-        <v>45542</v>
+      <c r="A44" s="3">
+        <v>45472</v>
       </c>
       <c r="B44" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C44" t="s">
         <v>47</v>
       </c>
       <c r="D44" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="2">
+        <v>45.904357736606926</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="4">
+        <v>45474</v>
+      </c>
+      <c r="B45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="2">
-        <v>21.577894032917253</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="3">
-        <v>45456</v>
-      </c>
-      <c r="B45" t="s">
-        <v>35</v>
-      </c>
-      <c r="C45" t="s">
-        <v>47</v>
-      </c>
-      <c r="D45" t="s">
-        <v>17</v>
-      </c>
       <c r="E45" s="2">
-        <v>11.907243878342793</v>
+        <v>32.529640875787123</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -1827,23 +1695,23 @@
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="4">
-        <v>45543</v>
+      <c r="A46" s="3">
+        <v>45478</v>
       </c>
       <c r="B46" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C46" t="s">
         <v>47</v>
       </c>
       <c r="D46" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E46" s="2">
-        <v>25.003529250849283</v>
+        <v>16.073972115983096</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46">
         <v>1</v>
@@ -1851,76 +1719,76 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="4">
-        <v>45450</v>
+        <v>45481</v>
       </c>
       <c r="B47" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C47" t="s">
         <v>47</v>
       </c>
       <c r="D47" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E47" s="2">
-        <v>182.33130768296445</v>
+        <v>10.705744648820099</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="3">
-        <v>45440</v>
+        <v>45486</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="C48" t="s">
         <v>47</v>
       </c>
       <c r="D48" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E48" s="2">
-        <v>123.23149154686199</v>
+        <v>28.990897890685307</v>
       </c>
       <c r="F48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G48">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="4">
-        <v>45379</v>
+        <v>45494</v>
       </c>
       <c r="B49" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C49" t="s">
         <v>47</v>
       </c>
       <c r="D49" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E49" s="2">
-        <v>91.115032457869006</v>
+        <v>126.59078627224213</v>
       </c>
       <c r="F49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="3">
-        <v>45368</v>
+        <v>45495</v>
       </c>
       <c r="B50" t="s">
         <v>8</v>
@@ -1932,7 +1800,7 @@
         <v>8</v>
       </c>
       <c r="E50" s="2">
-        <v>34.412227678898994</v>
+        <v>12.061717676004944</v>
       </c>
       <c r="F50">
         <v>1</v>
@@ -1943,56 +1811,56 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="4">
-        <v>45323</v>
+        <v>45499</v>
       </c>
       <c r="B51" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C51" t="s">
         <v>47</v>
       </c>
       <c r="D51" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E51" s="2">
-        <v>23.859230634878017</v>
+        <v>4.0793809055140491</v>
       </c>
       <c r="F51">
         <v>1</v>
       </c>
       <c r="G51">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="4">
-        <v>45353</v>
+      <c r="A52" s="3">
+        <v>45503</v>
       </c>
       <c r="B52" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C52" t="s">
         <v>47</v>
       </c>
       <c r="D52" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E52" s="2">
-        <v>8.4678212748500812</v>
+        <v>387.46481586504211</v>
       </c>
       <c r="F52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G52">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="3">
-        <v>45332</v>
+      <c r="A53" s="4">
+        <v>45510</v>
       </c>
       <c r="B53" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C53" t="s">
         <v>47</v>
@@ -2001,7 +1869,7 @@
         <v>16</v>
       </c>
       <c r="E53" s="2">
-        <v>24.677305430093984</v>
+        <v>3.8086864651546297</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -2011,8 +1879,8 @@
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="4">
-        <v>45575</v>
+      <c r="A54" s="3">
+        <v>45514</v>
       </c>
       <c r="B54" t="s">
         <v>12</v>
@@ -2024,7 +1892,7 @@
         <v>11</v>
       </c>
       <c r="E54" s="2">
-        <v>43.357284027160432</v>
+        <v>47.202743940079138</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -2035,30 +1903,30 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="4">
-        <v>45577</v>
+        <v>45515</v>
       </c>
       <c r="B55" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="C55" t="s">
         <v>47</v>
       </c>
       <c r="D55" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E55" s="2">
-        <v>24.960541772205787</v>
+        <v>45.542571114625908</v>
       </c>
       <c r="F55">
         <v>1</v>
       </c>
       <c r="G55">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="3">
-        <v>45578</v>
+        <v>45521</v>
       </c>
       <c r="B56" t="s">
         <v>8</v>
@@ -2070,7 +1938,7 @@
         <v>8</v>
       </c>
       <c r="E56" s="2">
-        <v>29.512426669497486</v>
+        <v>29.018191431636822</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -2080,69 +1948,69 @@
       </c>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="3">
-        <v>45402</v>
+      <c r="A57" s="4">
+        <v>45524</v>
       </c>
       <c r="B57" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="C57" t="s">
         <v>47</v>
       </c>
       <c r="D57" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E57" s="2">
-        <v>138.2147422166174</v>
+        <v>8.9102359077551156</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:7">
-      <c r="A58" s="4">
-        <v>45442</v>
+      <c r="A58" s="3">
+        <v>45527</v>
       </c>
       <c r="B58" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C58" t="s">
         <v>47</v>
       </c>
       <c r="D58" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E58" s="2">
-        <v>27.674824235526113</v>
+        <v>100.18836650895901</v>
       </c>
       <c r="F58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G58">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="4">
-        <v>45419</v>
+        <v>45528</v>
       </c>
       <c r="B59" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="C59" t="s">
         <v>47</v>
       </c>
       <c r="D59" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E59" s="2">
-        <v>25.568377219304327</v>
+        <v>39.268263806949975</v>
       </c>
       <c r="F59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -2150,22 +2018,22 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="3">
-        <v>45629</v>
+        <v>45536</v>
       </c>
       <c r="B60" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="C60" t="s">
         <v>47</v>
       </c>
       <c r="D60" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E60" s="2">
-        <v>10.924223157404425</v>
+        <v>13.768101260551122</v>
       </c>
       <c r="F60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G60">
         <v>1</v>
@@ -2173,33 +2041,33 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="4">
-        <v>45528</v>
+        <v>45540</v>
       </c>
       <c r="B61" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C61" t="s">
         <v>47</v>
       </c>
       <c r="D61" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E61" s="2">
-        <v>39.268263806949975</v>
+        <v>10.843589715267399</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G61">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="3">
-        <v>45536</v>
+        <v>45541</v>
       </c>
       <c r="B62" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C62" t="s">
         <v>47</v>
@@ -2208,7 +2076,7 @@
         <v>16</v>
       </c>
       <c r="E62" s="2">
-        <v>13.768101260551122</v>
+        <v>9.5459497283993091</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -2219,42 +2087,42 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="4">
-        <v>45393</v>
+        <v>45542</v>
       </c>
       <c r="B63" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C63" t="s">
         <v>47</v>
       </c>
       <c r="D63" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E63" s="2">
-        <v>3.6981094178656995</v>
+        <v>21.577894032917253</v>
       </c>
       <c r="F63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G63">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="4">
-        <v>45647</v>
+      <c r="A64" s="3">
+        <v>45543</v>
       </c>
       <c r="B64" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C64" t="s">
         <v>47</v>
       </c>
       <c r="D64" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E64" s="2">
-        <v>11.866231020207174</v>
+        <v>8.218023793872284</v>
       </c>
       <c r="F64">
         <v>0</v>
@@ -2264,11 +2132,11 @@
       </c>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65" s="3">
-        <v>45441</v>
+      <c r="A65" s="4">
+        <v>45543</v>
       </c>
       <c r="B65" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C65" t="s">
         <v>47</v>
@@ -2277,7 +2145,7 @@
         <v>16</v>
       </c>
       <c r="E65" s="2">
-        <v>8.1161906117480633</v>
+        <v>25.003529250849283</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -2288,22 +2156,22 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="3">
-        <v>45639</v>
+        <v>45547</v>
       </c>
       <c r="B66" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C66" t="s">
         <v>47</v>
       </c>
       <c r="D66" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E66" s="2">
-        <v>8.8561344087601057</v>
+        <v>19.033404509807344</v>
       </c>
       <c r="F66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G66">
         <v>1</v>
@@ -2311,68 +2179,68 @@
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="4">
-        <v>45406</v>
+        <v>45552</v>
       </c>
       <c r="B67" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C67" t="s">
         <v>47</v>
       </c>
       <c r="D67" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E67" s="2">
-        <v>59.465543593581948</v>
+        <v>45.124918956005892</v>
       </c>
       <c r="F67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G67">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="4">
-        <v>45639</v>
+      <c r="A68" s="3">
+        <v>45561</v>
       </c>
       <c r="B68" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C68" t="s">
         <v>47</v>
       </c>
       <c r="D68" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E68" s="2">
-        <v>26.00967141893349</v>
+        <v>65.067093202924426</v>
       </c>
       <c r="F68">
         <v>1</v>
       </c>
       <c r="G68">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" s="4">
-        <v>45494</v>
+        <v>45562</v>
       </c>
       <c r="B69" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="C69" t="s">
         <v>47</v>
       </c>
       <c r="D69" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E69" s="2">
-        <v>126.59078627224213</v>
+        <v>16.830074653529735</v>
       </c>
       <c r="F69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G69">
         <v>1</v>
@@ -2380,206 +2248,206 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="3">
-        <v>45317</v>
+        <v>45572</v>
       </c>
       <c r="B70" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C70" t="s">
         <v>47</v>
       </c>
       <c r="D70" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E70" s="2">
-        <v>546.34269896948445</v>
+        <v>18.005409657329089</v>
       </c>
       <c r="F70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G70">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:7">
-      <c r="A71" s="4">
-        <v>45510</v>
+      <c r="A71" s="3">
+        <v>45575</v>
       </c>
       <c r="B71" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C71" t="s">
         <v>47</v>
       </c>
       <c r="D71" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E71" s="2">
-        <v>3.8086864651546297</v>
+        <v>12.254949928414266</v>
       </c>
       <c r="F71">
         <v>1</v>
       </c>
       <c r="G71">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="4">
-        <v>45524</v>
+        <v>45575</v>
       </c>
       <c r="B72" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C72" t="s">
         <v>47</v>
       </c>
       <c r="D72" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E72" s="2">
-        <v>8.9102359077551156</v>
+        <v>43.357284027160432</v>
       </c>
       <c r="F72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G72">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="4">
-        <v>45440</v>
+        <v>45577</v>
       </c>
       <c r="B73" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="C73" t="s">
         <v>47</v>
       </c>
       <c r="D73" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E73" s="2">
-        <v>17.678550959111202</v>
+        <v>24.960541772205787</v>
       </c>
       <c r="F73">
         <v>1</v>
       </c>
       <c r="G73">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:7">
-      <c r="A74" s="4">
-        <v>45622</v>
+      <c r="A74" s="3">
+        <v>45578</v>
       </c>
       <c r="B74" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C74" t="s">
         <v>47</v>
       </c>
       <c r="D74" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E74" s="2">
-        <v>4.0966721465376077</v>
+        <v>29.512426669497486</v>
       </c>
       <c r="F74">
         <v>1</v>
       </c>
       <c r="G74">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" s="4">
-        <v>45628</v>
+        <v>45582</v>
       </c>
       <c r="B75" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C75" t="s">
         <v>47</v>
       </c>
       <c r="D75" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E75" s="2">
-        <v>5.4404930268114597</v>
+        <v>17.80165241729523</v>
       </c>
       <c r="F75">
         <v>1</v>
       </c>
       <c r="G75">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:7">
-      <c r="A76" s="4">
-        <v>45315</v>
+      <c r="A76" s="3">
+        <v>45593</v>
       </c>
       <c r="B76" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="C76" t="s">
         <v>47</v>
       </c>
       <c r="D76" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E76" s="2">
-        <v>18.209604367663978</v>
+        <v>47.674742913663458</v>
       </c>
       <c r="F76">
         <v>0</v>
       </c>
       <c r="G76">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:7">
-      <c r="A77" s="3">
-        <v>45472</v>
+      <c r="A77" s="4">
+        <v>45594</v>
       </c>
       <c r="B77" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C77" t="s">
         <v>47</v>
       </c>
       <c r="D77" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" s="2">
+        <v>53.524381510800161</v>
+      </c>
+      <c r="F77">
+        <v>1</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="3">
+        <v>45595</v>
+      </c>
+      <c r="B78" t="s">
+        <v>18</v>
+      </c>
+      <c r="C78" t="s">
+        <v>47</v>
+      </c>
+      <c r="D78" t="s">
         <v>11</v>
       </c>
-      <c r="E77" s="2">
-        <v>45.904357736606926</v>
-      </c>
-      <c r="F77">
-        <v>0</v>
-      </c>
-      <c r="G77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
-      <c r="A78" s="4">
-        <v>45396</v>
-      </c>
-      <c r="B78" t="s">
-        <v>8</v>
-      </c>
-      <c r="C78" t="s">
-        <v>47</v>
-      </c>
-      <c r="D78" t="s">
-        <v>8</v>
-      </c>
       <c r="E78" s="2">
-        <v>60.015682920995474</v>
+        <v>6.8664125929764026</v>
       </c>
       <c r="F78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -2587,19 +2455,19 @@
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="4">
-        <v>45454</v>
+        <v>45595</v>
       </c>
       <c r="B79" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="C79" t="s">
         <v>47</v>
       </c>
       <c r="D79" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E79" s="2">
-        <v>17.586058947264888</v>
+        <v>20.148806473862361</v>
       </c>
       <c r="F79">
         <v>0</v>
@@ -2609,66 +2477,66 @@
       </c>
     </row>
     <row r="80" spans="1:7">
-      <c r="A80" s="4">
-        <v>45582</v>
+      <c r="A80" s="3">
+        <v>45610</v>
       </c>
       <c r="B80" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C80" t="s">
         <v>47</v>
       </c>
       <c r="D80" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E80" s="2">
-        <v>17.80165241729523</v>
+        <v>23.409850623813977</v>
       </c>
       <c r="F80">
         <v>1</v>
       </c>
       <c r="G80">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" s="4">
-        <v>45594</v>
+        <v>45622</v>
       </c>
       <c r="B81" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C81" t="s">
         <v>47</v>
       </c>
       <c r="D81" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E81" s="2">
-        <v>53.524381510800161</v>
+        <v>4.0966721465376077</v>
       </c>
       <c r="F81">
         <v>1</v>
       </c>
       <c r="G81">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:7">
-      <c r="A82" s="4">
-        <v>45425</v>
+      <c r="A82" s="3">
+        <v>45623</v>
       </c>
       <c r="B82" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C82" t="s">
         <v>47</v>
       </c>
       <c r="D82" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E82" s="2">
-        <v>6.1133684042290115</v>
+        <v>18.750558620364448</v>
       </c>
       <c r="F82">
         <v>1</v>
@@ -2679,42 +2547,42 @@
     </row>
     <row r="83" spans="1:7">
       <c r="A83" s="3">
-        <v>45541</v>
+        <v>45627</v>
       </c>
       <c r="B83" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C83" t="s">
         <v>47</v>
       </c>
       <c r="D83" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E83" s="2">
-        <v>9.5459497283993091</v>
+        <v>55.806989867356052</v>
       </c>
       <c r="F83">
         <v>1</v>
       </c>
       <c r="G83">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:7">
-      <c r="A84" s="3">
-        <v>45644</v>
+      <c r="A84" s="4">
+        <v>45627</v>
       </c>
       <c r="B84" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="C84" t="s">
         <v>47</v>
       </c>
       <c r="D84" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E84" s="2">
-        <v>28.282964012150725</v>
+        <v>38.079442340158884</v>
       </c>
       <c r="F84">
         <v>0</v>
@@ -2725,7 +2593,7 @@
     </row>
     <row r="85" spans="1:7">
       <c r="A85" s="4">
-        <v>45499</v>
+        <v>45628</v>
       </c>
       <c r="B85" t="s">
         <v>27</v>
@@ -2737,7 +2605,7 @@
         <v>16</v>
       </c>
       <c r="E85" s="2">
-        <v>4.0793809055140491</v>
+        <v>5.4404930268114597</v>
       </c>
       <c r="F85">
         <v>1</v>
@@ -2748,33 +2616,33 @@
     </row>
     <row r="86" spans="1:7">
       <c r="A86" s="3">
-        <v>45521</v>
+        <v>45629</v>
       </c>
       <c r="B86" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="C86" t="s">
         <v>47</v>
       </c>
       <c r="D86" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E86" s="2">
-        <v>29.018191431636822</v>
+        <v>10.924223157404425</v>
       </c>
       <c r="F86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G86">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" s="4">
-        <v>45595</v>
+        <v>45632</v>
       </c>
       <c r="B87" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="C87" t="s">
         <v>47</v>
@@ -2783,99 +2651,99 @@
         <v>7</v>
       </c>
       <c r="E87" s="2">
-        <v>20.148806473862361</v>
+        <v>33.706145994917662</v>
       </c>
       <c r="F87">
         <v>0</v>
       </c>
       <c r="G87">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" s="3">
-        <v>45495</v>
+        <v>45639</v>
       </c>
       <c r="B88" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C88" t="s">
         <v>47</v>
       </c>
       <c r="D88" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E88" s="2">
-        <v>12.061717676004944</v>
+        <v>8.8561344087601057</v>
       </c>
       <c r="F88">
         <v>1</v>
       </c>
       <c r="G88">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:7">
-      <c r="A89" s="3">
-        <v>45468</v>
+      <c r="A89" s="4">
+        <v>45639</v>
       </c>
       <c r="B89" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C89" t="s">
         <v>47</v>
       </c>
       <c r="D89" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E89" s="2">
-        <v>26.169127192058014</v>
+        <v>26.00967141893349</v>
       </c>
       <c r="F89">
         <v>1</v>
       </c>
       <c r="G89">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" s="4">
-        <v>45336</v>
+        <v>45642</v>
       </c>
       <c r="B90" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C90" t="s">
         <v>47</v>
       </c>
       <c r="D90" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E90" s="2">
-        <v>4.1295821605673417</v>
+        <v>35.881275421039959</v>
       </c>
       <c r="F90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G90">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:7">
-      <c r="A91" s="4">
-        <v>45627</v>
+      <c r="A91" s="3">
+        <v>45642</v>
       </c>
       <c r="B91" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C91" t="s">
         <v>47</v>
       </c>
       <c r="D91" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E91" s="2">
-        <v>38.079442340158884</v>
+        <v>207.00141369968208</v>
       </c>
       <c r="F91">
         <v>0</v>
@@ -2886,10 +2754,10 @@
     </row>
     <row r="92" spans="1:7">
       <c r="A92" s="3">
-        <v>45380</v>
+        <v>45644</v>
       </c>
       <c r="B92" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C92" t="s">
         <v>47</v>
@@ -2898,7 +2766,7 @@
         <v>17</v>
       </c>
       <c r="E92" s="2">
-        <v>61.350532464411664</v>
+        <v>28.282964012150725</v>
       </c>
       <c r="F92">
         <v>0</v>
@@ -2909,10 +2777,10 @@
     </row>
     <row r="93" spans="1:7">
       <c r="A93" s="3">
-        <v>45610</v>
+        <v>45647</v>
       </c>
       <c r="B93" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C93" t="s">
         <v>47</v>
@@ -2921,7 +2789,7 @@
         <v>16</v>
       </c>
       <c r="E93" s="2">
-        <v>23.409850623813977</v>
+        <v>5.0872433310860332</v>
       </c>
       <c r="F93">
         <v>1</v>
@@ -2932,19 +2800,19 @@
     </row>
     <row r="94" spans="1:7">
       <c r="A94" s="4">
-        <v>45470</v>
+        <v>45647</v>
       </c>
       <c r="B94" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C94" t="s">
         <v>47</v>
       </c>
       <c r="D94" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E94" s="2">
-        <v>184.65116515446616</v>
+        <v>11.866231020207174</v>
       </c>
       <c r="F94">
         <v>0</v>
@@ -2955,10 +2823,10 @@
     </row>
     <row r="95" spans="1:7">
       <c r="A95" s="5">
-        <v>45451</v>
+        <v>45653</v>
       </c>
       <c r="B95" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C95" t="s">
         <v>47</v>
@@ -2967,7 +2835,7 @@
         <v>16</v>
       </c>
       <c r="E95" s="2">
-        <v>15.374193649330747</v>
+        <v>4.5444022945078419</v>
       </c>
       <c r="F95">
         <v>1</v>
@@ -2983,880 +2851,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3EB3251-4FC4-4EFB-A336-AF1B21393CF0}">
-  <dimension ref="A1:B95"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A95" sqref="A2:A95"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="9.140625" style="6"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3">
-        <v>45392</v>
-      </c>
-      <c r="B2" s="7">
-        <f ca="1">RAND()</f>
-        <v>0.85578244643325097</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="4">
-        <v>45389</v>
-      </c>
-      <c r="B3" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.25868480386181769</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3">
-        <v>45595</v>
-      </c>
-      <c r="B4" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.95256536777368939</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="3">
-        <v>45394</v>
-      </c>
-      <c r="B5" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.24570250096690072</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="4">
-        <v>45474</v>
-      </c>
-      <c r="B6" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.88926977601240798</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="3">
-        <v>45547</v>
-      </c>
-      <c r="B7" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.50973328972371734</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="4">
-        <v>45515</v>
-      </c>
-      <c r="B8" s="8">
-        <f ca="1">RAND()</f>
-        <v>8.7152480175947011E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="3">
-        <v>45395</v>
-      </c>
-      <c r="B9" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.83048609417028951</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="3">
-        <v>45322</v>
-      </c>
-      <c r="B10" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.61070733637547781</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="4">
-        <v>45642</v>
-      </c>
-      <c r="B11" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.38439401418439734</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="3">
-        <v>45478</v>
-      </c>
-      <c r="B12" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.71555605598590732</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="4">
-        <v>45395</v>
-      </c>
-      <c r="B13" s="8">
-        <f ca="1">RAND()</f>
-        <v>2.8660435720706423E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="4">
-        <v>45632</v>
-      </c>
-      <c r="B14" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.34920150066905342</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="4">
-        <v>45552</v>
-      </c>
-      <c r="B15" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.89805961479960439</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="3">
-        <v>45447</v>
-      </c>
-      <c r="B16" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.10632000241014761</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="4">
-        <v>45462</v>
-      </c>
-      <c r="B17" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.34985961417205869</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="4">
-        <v>45457</v>
-      </c>
-      <c r="B18" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.87909017080111329</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="3">
-        <v>45543</v>
-      </c>
-      <c r="B19" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.12682576385696909</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="3">
-        <v>45627</v>
-      </c>
-      <c r="B20" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.70161418122212371</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="3">
-        <v>45458</v>
-      </c>
-      <c r="B21" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.174092124976995</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="4">
-        <v>45540</v>
-      </c>
-      <c r="B22" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.85813713515690637</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="4">
-        <v>45653</v>
-      </c>
-      <c r="B23" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.92769661309063245</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="3">
-        <v>45514</v>
-      </c>
-      <c r="B24" s="8">
-        <f ca="1">RAND()</f>
-        <v>4.0457960526361192E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="3">
-        <v>45572</v>
-      </c>
-      <c r="B25" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.23119809439957317</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="3">
-        <v>45593</v>
-      </c>
-      <c r="B26" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.87364343202114336</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="3">
-        <v>45292</v>
-      </c>
-      <c r="B27" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.19930195534507456</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="3">
-        <v>45350</v>
-      </c>
-      <c r="B28" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.56908938877260018</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="3">
-        <v>45575</v>
-      </c>
-      <c r="B29" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.1834918878078533</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="3">
-        <v>45647</v>
-      </c>
-      <c r="B30" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.70276410732441319</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="4">
-        <v>45321</v>
-      </c>
-      <c r="B31" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.96973680072099011</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="3">
-        <v>45412</v>
-      </c>
-      <c r="B32" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.95695223136207519</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="4">
-        <v>45481</v>
-      </c>
-      <c r="B33" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.54494772659994861</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="3">
-        <v>45311</v>
-      </c>
-      <c r="B34" s="8">
-        <f ca="1">RAND()</f>
-        <v>8.5560096793153129E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="3">
-        <v>45503</v>
-      </c>
-      <c r="B35" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.6703306554177173</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="3">
-        <v>45561</v>
-      </c>
-      <c r="B36" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.82062941447455451</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="3">
-        <v>45642</v>
-      </c>
-      <c r="B37" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.8994579326794484</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="3">
-        <v>45423</v>
-      </c>
-      <c r="B38" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.62126540421724996</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="3">
-        <v>45623</v>
-      </c>
-      <c r="B39" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.28488955844280095</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="3">
-        <v>45527</v>
-      </c>
-      <c r="B40" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.77063095355079647</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="4">
-        <v>45311</v>
-      </c>
-      <c r="B41" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.23843633567143829</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="3">
-        <v>45486</v>
-      </c>
-      <c r="B42" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.15151387091237511</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="4">
-        <v>45562</v>
-      </c>
-      <c r="B43" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.94757273221392191</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="4">
-        <v>45542</v>
-      </c>
-      <c r="B44" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.57745097621284802</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="3">
-        <v>45456</v>
-      </c>
-      <c r="B45" s="8">
-        <f ca="1">RAND()</f>
-        <v>8.7774973824360725E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="4">
-        <v>45543</v>
-      </c>
-      <c r="B46" s="8">
-        <f ca="1">RAND()</f>
-        <v>8.8492998499789532E-3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="4">
-        <v>45450</v>
-      </c>
-      <c r="B47" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.25106612858976918</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="3">
-        <v>45440</v>
-      </c>
-      <c r="B48" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.92494608066473916</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="4">
-        <v>45379</v>
-      </c>
-      <c r="B49" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.13128715402125635</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="3">
-        <v>45368</v>
-      </c>
-      <c r="B50" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.9497266291189328</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="4">
-        <v>45323</v>
-      </c>
-      <c r="B51" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.89071685052303606</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="4">
-        <v>45353</v>
-      </c>
-      <c r="B52" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.71101741223270487</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="3">
-        <v>45332</v>
-      </c>
-      <c r="B53" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.30231207521674508</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="4">
-        <v>45575</v>
-      </c>
-      <c r="B54" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.16149597519477776</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="4">
-        <v>45577</v>
-      </c>
-      <c r="B55" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.10640268008457532</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="3">
-        <v>45578</v>
-      </c>
-      <c r="B56" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.34347492239365274</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="3">
-        <v>45402</v>
-      </c>
-      <c r="B57" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.1794364947339615</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="4">
-        <v>45442</v>
-      </c>
-      <c r="B58" s="8">
-        <f ca="1">RAND()</f>
-        <v>2.4024314216216092E-2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="4">
-        <v>45419</v>
-      </c>
-      <c r="B59" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.85943760866372065</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="3">
-        <v>45629</v>
-      </c>
-      <c r="B60" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.28042400160368075</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="4">
-        <v>45528</v>
-      </c>
-      <c r="B61" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.56636287417276066</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="3">
-        <v>45536</v>
-      </c>
-      <c r="B62" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.88044987314061718</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="4">
-        <v>45393</v>
-      </c>
-      <c r="B63" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.965979958880545</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="4">
-        <v>45647</v>
-      </c>
-      <c r="B64" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.96629138372225054</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="3">
-        <v>45441</v>
-      </c>
-      <c r="B65" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.35208131214473026</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="3">
-        <v>45639</v>
-      </c>
-      <c r="B66" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.34938823880436753</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="4">
-        <v>45406</v>
-      </c>
-      <c r="B67" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.66599102966258428</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="4">
-        <v>45639</v>
-      </c>
-      <c r="B68" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.36825600756529508</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="4">
-        <v>45494</v>
-      </c>
-      <c r="B69" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.99138484261872206</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="3">
-        <v>45317</v>
-      </c>
-      <c r="B70" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.47113421614946283</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="4">
-        <v>45510</v>
-      </c>
-      <c r="B71" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.24726097858480323</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="4">
-        <v>45524</v>
-      </c>
-      <c r="B72" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.64352932889279424</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="4">
-        <v>45440</v>
-      </c>
-      <c r="B73" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.79308458863630349</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="4">
-        <v>45622</v>
-      </c>
-      <c r="B74" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.40311941701152443</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="4">
-        <v>45628</v>
-      </c>
-      <c r="B75" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.39053456248145868</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="4">
-        <v>45315</v>
-      </c>
-      <c r="B76" s="8">
-        <f ca="1">RAND()</f>
-        <v>4.6156534315552666E-2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="3">
-        <v>45472</v>
-      </c>
-      <c r="B77" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.77887780156762576</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="4">
-        <v>45396</v>
-      </c>
-      <c r="B78" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.57634000273619357</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="4">
-        <v>45454</v>
-      </c>
-      <c r="B79" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.58542217707576805</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="A80" s="4">
-        <v>45582</v>
-      </c>
-      <c r="B80" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.68824709944652485</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="4">
-        <v>45594</v>
-      </c>
-      <c r="B81" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.18753799905952051</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="4">
-        <v>45425</v>
-      </c>
-      <c r="B82" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.40411463989093455</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="3">
-        <v>45541</v>
-      </c>
-      <c r="B83" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.65503260925826423</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="3">
-        <v>45644</v>
-      </c>
-      <c r="B84" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.23173286309322583</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="4">
-        <v>45499</v>
-      </c>
-      <c r="B85" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.67741797697289896</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="3">
-        <v>45521</v>
-      </c>
-      <c r="B86" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.85323660787144751</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="4">
-        <v>45595</v>
-      </c>
-      <c r="B87" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.3188585614040218</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="A88" s="3">
-        <v>45495</v>
-      </c>
-      <c r="B88" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.80843259148070079</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="3">
-        <v>45468</v>
-      </c>
-      <c r="B89" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.72494968688368633</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="4">
-        <v>45336</v>
-      </c>
-      <c r="B90" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.44626805547395232</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="4">
-        <v>45627</v>
-      </c>
-      <c r="B91" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.17731858176842152</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="3">
-        <v>45380</v>
-      </c>
-      <c r="B92" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.39533969461135743</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="3">
-        <v>45610</v>
-      </c>
-      <c r="B93" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.628708744239313</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" s="4">
-        <v>45470</v>
-      </c>
-      <c r="B94" s="8">
-        <f ca="1">RAND()</f>
-        <v>0.46037730855780323</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" s="5">
-        <v>45451</v>
-      </c>
-      <c r="B95" s="9">
-        <f ca="1">RAND()</f>
-        <v>0.39623598571142937</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>